<commit_message>
Added negative test cases for auth
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/user.xlsx
+++ b/src/main/resources/excel/user.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="10">
   <si>
     <t>firstName</t>
   </si>
@@ -813,6 +813,188 @@
         <v>9</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>